<commit_message>
Add some changes in TableSQL and DiagramTables
</commit_message>
<xml_diff>
--- a/DDL/DiagramTables.xlsx
+++ b/DDL/DiagramTables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maria\git\OncologyDataBase\DDL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agarc\git\OncologyDataBase\DDL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0B3B0A-AEFB-47E6-B477-E045D62C84EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417D1F04-F681-448A-9A2A-85F66A89010E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="71">
   <si>
     <t>PATIENT</t>
   </si>
@@ -81,9 +81,6 @@
     <t>TREATMENT</t>
   </si>
   <si>
-    <t> </t>
-  </si>
-  <si>
     <t>MEDICAL EXAMINATIONS</t>
   </si>
   <si>
@@ -159,9 +156,6 @@
     <t>Lung</t>
   </si>
   <si>
-    <t>Chest</t>
-  </si>
-  <si>
     <t>Stomach</t>
   </si>
   <si>
@@ -211,6 +205,45 @@
   </si>
   <si>
     <t> 3</t>
+  </si>
+  <si>
+    <t>High fever</t>
+  </si>
+  <si>
+    <t>Breathing difficulties</t>
+  </si>
+  <si>
+    <t> Abdomen pain</t>
+  </si>
+  <si>
+    <t>PET</t>
+  </si>
+  <si>
+    <t>MRI</t>
+  </si>
+  <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>Biopsy</t>
+  </si>
+  <si>
+    <t>Cancer</t>
+  </si>
+  <si>
+    <t>No cancer</t>
+  </si>
+  <si>
+    <t>Breast</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Medium</t>
   </si>
 </sst>
 </file>
@@ -478,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -542,9 +575,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -884,30 +914,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35:D35"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.88671875" customWidth="1"/>
-    <col min="2" max="2" width="25.109375" customWidth="1"/>
+    <col min="1" max="1" width="9.90625" customWidth="1"/>
+    <col min="2" max="2" width="25.08984375" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" customWidth="1"/>
+    <col min="4" max="4" width="17.81640625" customWidth="1"/>
+    <col min="5" max="5" width="12.90625" customWidth="1"/>
+    <col min="6" max="6" width="14.08984375" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
-    <col min="8" max="8" width="19.6640625" customWidth="1"/>
-    <col min="9" max="9" width="15.109375" customWidth="1"/>
-    <col min="10" max="11" width="10.77734375" customWidth="1"/>
+    <col min="8" max="8" width="19.6328125" customWidth="1"/>
+    <col min="9" max="9" width="15.08984375" customWidth="1"/>
+    <col min="10" max="11" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B3" s="15" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B4" s="14" t="s">
         <v>1</v>
       </c>
@@ -935,111 +965,119 @@
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B5" s="16">
         <v>1</v>
       </c>
       <c r="C5" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="16" t="s">
-        <v>29</v>
-      </c>
       <c r="E5" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F5" s="21">
         <v>37227</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" s="19"/>
+        <v>37</v>
+      </c>
+      <c r="I5" s="19">
+        <v>1</v>
+      </c>
       <c r="J5" s="13"/>
       <c r="K5" s="13"/>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B6" s="16">
         <v>2</v>
       </c>
       <c r="C6" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="16" t="s">
-        <v>31</v>
-      </c>
       <c r="E6" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F6" s="21">
         <v>37196</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="19"/>
+        <v>38</v>
+      </c>
+      <c r="I6" s="19">
+        <v>2</v>
+      </c>
       <c r="J6" s="13"/>
       <c r="K6" s="13"/>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B7" s="16">
         <v>3</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F7" s="21">
         <v>36924</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="I7" s="19"/>
+        <v>38</v>
+      </c>
+      <c r="I7" s="19">
+        <v>2</v>
+      </c>
       <c r="J7" s="13"/>
       <c r="K7" s="13"/>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B8" s="17">
         <v>4</v>
       </c>
       <c r="C8" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="E8" s="17" t="s">
         <v>34</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>35</v>
       </c>
       <c r="F8" s="22">
         <v>35839</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="I8" s="20"/>
+        <v>37</v>
+      </c>
+      <c r="I8" s="20">
+        <v>4</v>
+      </c>
       <c r="J8" s="13"/>
       <c r="K8" s="13"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
       <c r="D9" s="13"/>
@@ -1051,7 +1089,7 @@
       <c r="J9" s="13"/>
       <c r="K9" s="13"/>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B11" s="15" t="s">
         <v>9</v>
       </c>
@@ -1059,94 +1097,134 @@
         <v>10</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B12" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="34" t="s">
+      <c r="D12" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="35" t="s">
+      <c r="G12" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="36" t="s">
+      <c r="H12" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="34" t="s">
+      <c r="J12" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="K12" s="34" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="K12" s="33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B13" s="16">
         <v>1</v>
       </c>
       <c r="C13" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="32">
+        <v>2</v>
+      </c>
+      <c r="G13" s="16">
+        <v>1</v>
+      </c>
+      <c r="H13" s="16">
+        <v>4</v>
+      </c>
+      <c r="I13" s="26"/>
+      <c r="J13" s="27">
+        <v>4</v>
+      </c>
+      <c r="K13" s="27">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B14" s="16">
+        <v>2</v>
+      </c>
+      <c r="C14" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="33"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="27"/>
-      <c r="K13" s="27"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B14" s="16">
-        <v>2</v>
-      </c>
-      <c r="C14" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
+      <c r="D14" s="16">
+        <v>2</v>
+      </c>
+      <c r="G14" s="16">
+        <v>2</v>
+      </c>
+      <c r="H14" s="16">
+        <v>1</v>
+      </c>
       <c r="I14" s="26"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="J14" s="27">
+        <v>1</v>
+      </c>
+      <c r="K14" s="27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B15" s="16">
         <v>3</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
+        <v>67</v>
+      </c>
+      <c r="D15" s="16">
+        <v>4</v>
+      </c>
+      <c r="G15" s="16">
+        <v>3</v>
+      </c>
+      <c r="H15" s="16">
+        <v>1</v>
+      </c>
       <c r="I15" s="26"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="27"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="J15" s="27">
+        <v>1</v>
+      </c>
+      <c r="K15" s="27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B16" s="16">
         <v>4</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
+        <v>41</v>
+      </c>
+      <c r="D16" s="16">
+        <v>2</v>
+      </c>
+      <c r="G16" s="16">
+        <v>4</v>
+      </c>
+      <c r="H16" s="16">
+        <v>3</v>
+      </c>
       <c r="I16" s="26"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="J16" s="27">
+        <v>3</v>
+      </c>
+      <c r="K16" s="27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" s="6" t="s">
         <v>14</v>
       </c>
@@ -1154,146 +1232,150 @@
         <v>12</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E20" s="30" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" s="28">
         <v>1</v>
       </c>
       <c r="C21" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" s="30"/>
-      <c r="E21" s="30" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="D21" s="21">
+        <v>42318</v>
+      </c>
+      <c r="E21" s="30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B22" s="28">
         <v>2</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="31"/>
-      <c r="E22" s="30" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="D22" s="21">
+        <v>39163</v>
+      </c>
+      <c r="E22" s="30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B23" s="28">
         <v>3</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="30" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="30" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="28.8" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="D23" s="21">
+        <v>37149</v>
+      </c>
+      <c r="E23" s="30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="29" x14ac:dyDescent="0.35">
       <c r="B24" s="28">
         <v>4</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" s="30" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="21">
+        <v>37203</v>
+      </c>
+      <c r="E24" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="31" t="s">
         <v>16</v>
-      </c>
-      <c r="E24" s="30" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="32" t="s">
-        <v>17</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B27" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="37" t="s">
+      <c r="C27" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="37" t="s">
+      <c r="D27" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="E27" s="37" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B28" s="28">
         <v>1</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="D28" s="29" t="s">
-        <v>16</v>
+        <v>61</v>
+      </c>
+      <c r="D28" s="21">
+        <v>42311</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B29" s="28">
         <v>2</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="29" t="s">
-        <v>16</v>
+        <v>62</v>
+      </c>
+      <c r="D29" s="21">
+        <v>37142</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B30" s="28">
         <v>3</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" s="29" t="s">
-        <v>16</v>
+        <v>63</v>
+      </c>
+      <c r="D30" s="21">
+        <v>39147</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B31" s="28">
         <v>4</v>
       </c>
       <c r="C31" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="D31" s="29" t="s">
-        <v>16</v>
+        <v>64</v>
+      </c>
+      <c r="D31" s="21">
+        <v>37196</v>
       </c>
       <c r="E31" s="29" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B34" s="32" t="s">
-        <v>20</v>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B34" s="31" t="s">
+        <v>19</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -1301,73 +1383,103 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B35" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="38" t="s">
+      <c r="D35" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I35" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D35" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="H35" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="I35" s="5" t="s">
+      <c r="J35" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="J35" s="11" t="s">
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B36" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D36" s="16">
+        <v>1</v>
+      </c>
+      <c r="H36" s="16">
+        <v>1</v>
+      </c>
+      <c r="I36" s="16">
+        <v>3</v>
+      </c>
+      <c r="J36" s="16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="B37" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" s="16">
+        <v>2</v>
+      </c>
+      <c r="H37" s="16">
+        <v>2</v>
+      </c>
+      <c r="I37" s="16">
+        <v>3</v>
+      </c>
+      <c r="J37" s="16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B38" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D38" s="16">
+        <v>2</v>
+      </c>
+      <c r="H38" s="16">
+        <v>3</v>
+      </c>
+      <c r="I38" s="16">
+        <v>1</v>
+      </c>
+      <c r="J38" s="16" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="H39" s="16">
+        <v>4</v>
+      </c>
+      <c r="I39" s="16">
+        <v>2</v>
+      </c>
+      <c r="J39" s="16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B41" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B36" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B37" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B38" s="28" t="s">
-        <v>59</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B41" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B42" s="14" t="s">
         <v>8</v>
       </c>
@@ -1375,51 +1487,51 @@
         <v>12</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B43" s="16">
         <v>1</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B44" s="16">
         <v>2</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B45" s="16">
         <v>3</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B46" s="16">
         <v>4</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes in method diagnosis
</commit_message>
<xml_diff>
--- a/DDL/DiagramTables.xlsx
+++ b/DDL/DiagramTables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agarc\git\OncologyDataBase\DDL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417D1F04-F681-448A-9A2A-85F66A89010E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00509B3E-2335-431B-BE74-46778CE503A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="72">
   <si>
     <t>PATIENT</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>Medium</t>
+  </si>
+  <si>
+    <t>patient_id</t>
   </si>
 </sst>
 </file>
@@ -511,7 +514,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -596,6 +599,9 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -914,8 +920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1219,12 +1225,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B19" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B20" s="6" t="s">
         <v>14</v>
       </c>
@@ -1238,7 +1244,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B21" s="28">
         <v>1</v>
       </c>
@@ -1252,7 +1258,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B22" s="28">
         <v>2</v>
       </c>
@@ -1266,7 +1272,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B23" s="28">
         <v>3</v>
       </c>
@@ -1280,7 +1286,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B24" s="28">
         <v>4</v>
       </c>
@@ -1294,8 +1300,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="26" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="31" t="s">
         <v>16</v>
       </c>
@@ -1303,7 +1309,7 @@
       <c r="D26" s="3"/>
       <c r="E26" s="4"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B27" s="6" t="s">
         <v>13</v>
       </c>
@@ -1316,8 +1322,11 @@
       <c r="E27" s="36" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F27" s="38" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B28" s="28">
         <v>1</v>
       </c>
@@ -1330,8 +1339,11 @@
       <c r="E28" s="29" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F28" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B29" s="28">
         <v>2</v>
       </c>
@@ -1344,8 +1356,11 @@
       <c r="E29" s="29" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F29" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B30" s="28">
         <v>3</v>
       </c>
@@ -1358,8 +1373,11 @@
       <c r="E30" s="29" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="F30" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B31" s="28">
         <v>4</v>
       </c>
@@ -1371,6 +1389,9 @@
       </c>
       <c r="E31" s="29" t="s">
         <v>65</v>
+      </c>
+      <c r="F31" s="29">
+        <v>6</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.35">
@@ -1390,9 +1411,7 @@
       <c r="C35" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="D35" s="35" t="s">
-        <v>13</v>
-      </c>
+      <c r="D35" s="35"/>
       <c r="H35" s="8" t="s">
         <v>1</v>
       </c>
@@ -1410,9 +1429,7 @@
       <c r="C36" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D36" s="16">
-        <v>1</v>
-      </c>
+      <c r="D36" s="16"/>
       <c r="H36" s="16">
         <v>1</v>
       </c>
@@ -1430,9 +1447,7 @@
       <c r="C37" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D37" s="16">
-        <v>2</v>
-      </c>
+      <c r="D37" s="16"/>
       <c r="H37" s="16">
         <v>2</v>
       </c>
@@ -1450,9 +1465,7 @@
       <c r="C38" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="D38" s="16">
-        <v>2</v>
-      </c>
+      <c r="D38" s="16"/>
       <c r="H38" s="16">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
java fx, DTD and SQL tables
</commit_message>
<xml_diff>
--- a/DDL/DiagramTables.xlsx
+++ b/DDL/DiagramTables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agarc\git\OncologyDataBase\DDL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00509B3E-2335-431B-BE74-46778CE503A8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A258F9-7DBE-4397-87BF-B529712BFD2B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="73">
   <si>
     <t>PATIENT</t>
   </si>
@@ -247,6 +247,9 @@
   </si>
   <si>
     <t>patient_id</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -920,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1117,7 +1120,7 @@
         <v>13</v>
       </c>
       <c r="G12" s="34" t="s">
-        <v>11</v>
+        <v>72</v>
       </c>
       <c r="H12" s="35" t="s">
         <v>14</v>

</xml_diff>